<commit_message>
Done Systeminfo and Close Button
</commit_message>
<xml_diff>
--- a/system_overview.xlsx
+++ b/system_overview.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinhak\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinhak\Downloads\New folder (7)\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96DF71B-A87D-4F12-B804-CA99602787ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175A6FD9-B2F7-48C3-807D-BE8725583693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>SECTION</t>
   </si>
@@ -495,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,181 +698,6 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>